<commit_message>
criação do arquivo app.py com o metodo read_excel e alteração arquivo main.py para metodo ExcelFile
</commit_message>
<xml_diff>
--- a/planilhas/CCA.FER.xlsx
+++ b/planilhas/CCA.FER.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57351724920\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\OneDrive\Documentos\GitHub\analisadorPlanilhas\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4415525A-FB26-4BB9-80D6-0DA663FB881A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unidade XXX" sheetId="1" r:id="rId1"/>
@@ -19,28 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>UFSC</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -173,7 +163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,10 +257,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -569,11 +555,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implementação da coleção com numero de linhas de cada coluna
</commit_message>
<xml_diff>
--- a/planilhas/CCA.FER.xlsx
+++ b/planilhas/CCA.FER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\OneDrive\Documentos\GitHub\analisadorPlanilhas\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4415525A-FB26-4BB9-80D6-0DA663FB881A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888A575A-D726-4D30-BFC2-6AE7423CCE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="29">
   <si>
     <t>N. Patrimônio</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>S/N°</t>
+  </si>
+  <si>
+    <t>SimLuana</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>

</xml_diff>